<commit_message>
finished with code for holidays in stockholm
</commit_message>
<xml_diff>
--- a/Holidays/SkollovStockholm.xlsx
+++ b/Holidays/SkollovStockholm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svantepihl/Documents/R/CarFires/Holidays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526FA1D9-D150-9647-A5EC-D115D76645E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF7B929-1C16-1F47-A20E-AE6F984F6D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,10 +657,10 @@
   <dimension ref="A1:M1026"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomRight" activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3422,7 +3422,7 @@
         <v>43044</v>
       </c>
       <c r="M67" s="9">
-        <v>2599788</v>
+        <v>43091</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="13" x14ac:dyDescent="0.15">
@@ -3682,7 +3682,7 @@
         <v>58</v>
       </c>
       <c r="D74" s="8">
-        <v>371462</v>
+        <v>42744</v>
       </c>
       <c r="E74" s="8">
         <v>42793</v>

</xml_diff>